<commit_message>
creae export in purchased order
</commit_message>
<xml_diff>
--- a/app/webroot/img/purchased_item.xlsx
+++ b/app/webroot/img/purchased_item.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20610" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,14 +109,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,91 +433,91 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="13.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
-    <col min="8" max="8" width="14.5703125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="5"/>
+    <col min="1" max="1" width="20.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="20" style="7" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="14.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>